<commit_message>
Update model's physical parameters
</commit_message>
<xml_diff>
--- a/parameters2.xlsx
+++ b/parameters2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carter\Desktop\subbots\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DAFB127-AEA3-422E-9C99-B0C13F4AC648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4B68E-F2C0-493F-8DB2-15E403CDA900}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8511" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>Mass</t>
   </si>
@@ -307,6 +307,21 @@
   </si>
   <si>
     <t>m^2</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>DIM_X</t>
+  </si>
+  <si>
+    <t>DIM_Y</t>
+  </si>
+  <si>
+    <t>DIM_Z</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
 </sst>
 </file>
@@ -493,24 +508,6 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -547,12 +544,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -948,647 +963,712 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9">
+      <c r="B1" s="35"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3">
         <v>24.5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="3">
         <v>1.704717</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="3">
         <v>1.539285</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="3">
         <v>1.6030800000000001</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="6">
         <f>D1*1.01*9.81</f>
         <v>242.74845000000002</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="10">
         <v>-3.73E-2</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="10">
         <v>0</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="13">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="13">
         <v>0.17</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="15">
         <f>Sheet2!E13</f>
         <v>41.756999999999991</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="16">
         <f>Sheet2!E21</f>
         <v>103.38959999999999</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="17">
         <f>Sheet2!E27</f>
         <v>72.575999999999993</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="18">
         <f>2/3*0.6^3*D12</f>
         <v>6.0130079999999984</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="18">
         <f>2/3*0.6^3*D13</f>
         <v>14.888102399999998</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="18">
         <f>2/3*0.6^3*D14</f>
         <v>10.450943999999998</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="3">
         <v>0</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="10">
         <v>0</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="10">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="10">
         <v>-0.06</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="20" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="10">
         <v>0</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="10">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="10">
         <v>0</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="10">
         <v>0</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="13">
         <v>0</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="20">
         <v>0</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="20" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="22">
         <v>0.27300000000000002</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="13" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="30">
+      <c r="D29" s="24">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="20">
         <v>0</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="20" t="s">
+      <c r="A31" s="32"/>
+      <c r="B31" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="22">
         <v>0.315</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="13" t="s">
+      <c r="A32" s="32"/>
+      <c r="B32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="24">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="E32" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="22">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A34" s="5"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="18" t="s">
+    <row r="34" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A34" s="33"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="22">
         <v>2.67</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:6" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="15" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="13">
         <v>0.14699999999999999</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="18" t="s">
+    <row r="36" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A36" s="34"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="10">
         <v>3.2</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="28">
         <v>0.109066</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A38" s="35"/>
-      <c r="B38" s="17" t="s">
+      <c r="F37" s="28">
+        <v>0.230487</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="28">
+        <v>0.22428799999999999</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="28">
+        <v>0.22428799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
+      <c r="B39" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="28">
         <v>0.230487</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E39" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A39" s="35"/>
-      <c r="B39" s="17" t="s">
+      <c r="F39" s="28">
+        <v>0.109066</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A40" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="28">
+        <v>806.45</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="28">
+        <v>330.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="28">
+        <v>419.1</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="28">
+        <v>419.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="36">
-        <v>0.22428799999999999</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A40" s="33" t="s">
+      <c r="C42" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="28">
+        <v>330.2</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="28">
+        <v>806.45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A43" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="31" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D43" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E43" s="4" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1607,58 +1687,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="4">
         <v>0.3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="A2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="4">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="4">
         <v>0.87</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
       <c r="E5">
@@ -1667,16 +1747,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="4">
         <v>0.63</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6">
@@ -1685,16 +1765,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="4">
         <v>0.42</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="4">
         <v>2</v>
       </c>
       <c r="E7">
@@ -1703,17 +1783,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C8">
         <f>(0.91+0.42)/2</f>
         <v>0.66500000000000004</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8">
@@ -1722,16 +1802,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="4">
         <v>0.02</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="4">
         <v>1.2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9">
@@ -1740,16 +1820,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>1.3</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10">
@@ -1758,16 +1838,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="4">
         <v>1.6E-2</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>1.5</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11">
@@ -1776,7 +1856,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E13">
@@ -1785,38 +1865,38 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="26" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="4">
         <v>0.14699999999999999</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="4">
         <v>1.1200000000000001</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17">
@@ -1825,16 +1905,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="4">
         <v>5.5E-2</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="4">
         <v>0.68</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18">
@@ -1843,17 +1923,17 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B19">
         <f>0.09*0.06</f>
         <v>5.3999999999999994E-3</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="4">
         <v>0.63</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="4">
         <v>1</v>
       </c>
       <c r="E19">
@@ -1862,7 +1942,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E21">
@@ -1871,38 +1951,38 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="4">
         <v>0.216</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="4">
         <v>1.1200000000000001</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25">
@@ -1911,7 +1991,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E27">

</xml_diff>

<commit_message>
Implement model.m for comparing linear and non-linear models. Rotational and linear inertias used in non-linear ddot function. Placeholder values used for lin and quad friction
</commit_message>
<xml_diff>
--- a/parameters2.xlsx
+++ b/parameters2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carter\Desktop\subbots\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4B68E-F2C0-493F-8DB2-15E403CDA900}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C798905-4260-4A38-9F2A-6471E086D314}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8511" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="101">
   <si>
     <t>Mass</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>Added Mass</t>
+  </si>
+  <si>
+    <t>MA_X</t>
+  </si>
+  <si>
+    <t>MA_Y</t>
+  </si>
+  <si>
+    <t>MA_Z</t>
   </si>
 </sst>
 </file>
@@ -506,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -548,6 +560,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,18 +577,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -963,10 +976,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -978,7 +991,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -995,7 +1008,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1023,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A4" s="35"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1025,10 +1038,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1054,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1058,7 +1071,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1073,7 +1086,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A8" s="36"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1101,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1105,7 +1118,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1133,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1148,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1153,7 +1166,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1182,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1198,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1203,7 +1216,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="14" t="s">
         <v>7</v>
       </c>
@@ -1219,7 +1232,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
@@ -1235,7 +1248,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="31" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1252,7 +1265,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A19" s="36"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="14" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1280,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1295,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1299,7 +1312,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A22" s="33"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="14" t="s">
         <v>7</v>
       </c>
@@ -1314,7 +1327,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A23" s="33"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="7" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1342,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1346,7 +1359,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A25" s="33"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="14" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1374,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A26" s="33"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
@@ -1376,7 +1389,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="34" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1393,7 +1406,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="14" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1421,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A29" s="31"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1436,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="35" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1440,7 +1453,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A31" s="32"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="14" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +1468,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1483,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="30" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1"/>
@@ -1485,7 +1498,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A34" s="33"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="7"/>
       <c r="C34" s="12" t="s">
         <v>54</v>
@@ -1498,7 +1511,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="36" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="1"/>
@@ -1513,7 +1526,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A36" s="34"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="7"/>
       <c r="C36" s="12" t="s">
         <v>58</v>
@@ -1638,37 +1651,87 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="28">
+        <v>12.834</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="37"/>
+    </row>
+    <row r="44" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="28">
+        <v>17.329499999999999</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="37"/>
+    </row>
+    <row r="45" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="28">
+        <v>21.937100000000001</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="37"/>
+    </row>
+    <row r="46" spans="1:6" ht="14.15" x14ac:dyDescent="0.35">
+      <c r="A46" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="25" t="s">
+      <c r="B46" s="33"/>
+      <c r="C46" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D46" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>